<commit_message>
Adding support for RedBee10 JSON
</commit_message>
<xml_diff>
--- a/epg-ingest/xls/EPG Mappings.xlsx
+++ b/epg-ingest/xls/EPG Mappings.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anders/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anders/git/emp/EMP-api/epg-ingest/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F1AEC5-C392-884B-9A04-9D7D074242C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51128DC3-E2FB-0B44-98CC-DE64EDD42039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1120" windowWidth="33440" windowHeight="22360" activeTab="2" xr2:uid="{5F35A65C-7244-4948-9085-0025D1C0981F}"/>
+    <workbookView xWindow="720" yWindow="1380" windowWidth="33440" windowHeight="22360" xr2:uid="{5F35A65C-7244-4948-9085-0025D1C0981F}"/>
   </bookViews>
   <sheets>
     <sheet name="EPG Datamodel" sheetId="1" r:id="rId1"/>
     <sheet name="TVAnytime" sheetId="2" r:id="rId2"/>
     <sheet name="XML TV" sheetId="3" r:id="rId3"/>
     <sheet name="CD API" sheetId="4" r:id="rId4"/>
+    <sheet name="RedBee10 (json)" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="247">
   <si>
     <t>Channel</t>
   </si>
@@ -664,6 +665,117 @@
   </si>
   <si>
     <t>Titles, descriptions, images are grouped by langauge.</t>
+  </si>
+  <si>
+    <t>schedule.start</t>
+  </si>
+  <si>
+    <t>schedule.end</t>
+  </si>
+  <si>
+    <t>schedule.programs</t>
+  </si>
+  <si>
+    <t>schedule.programs.programId</t>
+  </si>
+  <si>
+    <t>schedule.programs.assetId</t>
+  </si>
+  <si>
+    <t>schedule.programs.title</t>
+  </si>
+  <si>
+    <t>schedule.programs.publicStart</t>
+  </si>
+  <si>
+    <t>schedule.programs.publicEnd</t>
+  </si>
+  <si>
+    <t>schedule.programs.actualEnd</t>
+  </si>
+  <si>
+    <t>schedule.programs.actualStart</t>
+  </si>
+  <si>
+    <t>Right now there is no asset section in JSON EPG. Might be added later to support more asset information.</t>
+  </si>
+  <si>
+    <t>Asset purge date</t>
+  </si>
+  <si>
+    <t>schedule.program.assetPurgeDate</t>
+  </si>
+  <si>
+    <t>This is a new data element that is not yet supported internally in the platform. But we think we will at some point.</t>
+  </si>
+  <si>
+    <t>Picked up from program section as described above</t>
+  </si>
+  <si>
+    <t>Currently we do not support any localised section. Will be added later when needed.</t>
+  </si>
+  <si>
+    <t>schedule.program.publication.id</t>
+  </si>
+  <si>
+    <t>schedule.program.publication.visibleFrom</t>
+  </si>
+  <si>
+    <t>schedule.program.publication.start</t>
+  </si>
+  <si>
+    <t>schedule.program.publication.end</t>
+  </si>
+  <si>
+    <t>schedule.program.publication.contractId</t>
+  </si>
+  <si>
+    <t>schedule.program.publication.products</t>
+  </si>
+  <si>
+    <t>Geo blocking</t>
+  </si>
+  <si>
+    <t>Block VPN</t>
+  </si>
+  <si>
+    <t>Allowed Countries</t>
+  </si>
+  <si>
+    <t>Blocked Countries</t>
+  </si>
+  <si>
+    <t>schedule.program.publication.geoBlocking.blockVpn</t>
+  </si>
+  <si>
+    <t>schedule.program.publication.geoBlocking.allowedCountries</t>
+  </si>
+  <si>
+    <t>schedule.program.publication.geoBlocking.blockedCountries</t>
+  </si>
+  <si>
+    <t>Currenlty only supported here in RedBee10 json</t>
+  </si>
+  <si>
+    <t>Should we block VPNs?</t>
+  </si>
+  <si>
+    <t>Allowed countries in a geo blocking</t>
+  </si>
+  <si>
+    <t>Blocked countries in a geo blocking</t>
+  </si>
+  <si>
+    <t>Geo blocking can be added to a publication. Not available for all formats.</t>
+  </si>
+  <si>
+    <t>Should VPNs be blocked</t>
+  </si>
+  <si>
+    <t>Allowed countries when geo blocking is used.</t>
+  </si>
+  <si>
+    <t>Blocked countries when geo blocking is used</t>
   </si>
 </sst>
 </file>
@@ -816,7 +928,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -826,9 +938,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -840,16 +949,11 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1169,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42007D5-98B7-6F48-9081-76F8A481BB2F}">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1185,13 +1289,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="17">
       <c r="A2" s="3" t="s">
@@ -1263,13 +1367,13 @@
       <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" ht="26">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:5" ht="17">
       <c r="A10" s="3" t="s">
@@ -1407,18 +1511,18 @@
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="18"/>
+      <c r="A23" s="16"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="10"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" ht="25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" ht="17">
       <c r="A25" s="3" t="s">
@@ -1429,7 +1533,7 @@
       <c r="D25" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="9" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1442,7 +1546,7 @@
       <c r="D26" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1453,7 +1557,7 @@
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1466,7 +1570,7 @@
       <c r="D28" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1479,7 +1583,7 @@
       <c r="D29" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="9" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1492,7 +1596,7 @@
       <c r="D30" s="7">
         <v>1</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1505,7 +1609,7 @@
       <c r="D31" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1518,7 +1622,7 @@
       <c r="D32" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="9" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1531,7 +1635,7 @@
       <c r="D33" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1544,7 +1648,7 @@
       <c r="D34" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="9" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1557,7 +1661,7 @@
       <c r="D35" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="9" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1568,7 +1672,7 @@
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="9" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1581,7 +1685,7 @@
       <c r="D37" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="9" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1594,7 +1698,7 @@
       <c r="D38" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="9" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1605,7 +1709,7 @@
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="9" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1618,7 +1722,7 @@
       <c r="D40" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="9" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1631,7 +1735,7 @@
       <c r="D41" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="9" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1644,7 +1748,7 @@
       <c r="D42" s="7">
         <v>12</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="9" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1655,7 +1759,7 @@
       <c r="B43" s="4"/>
       <c r="C43" s="5"/>
       <c r="D43" s="6"/>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="9" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1668,7 +1772,7 @@
       <c r="D44" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="9" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1681,7 +1785,7 @@
       <c r="D45" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="9" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1694,7 +1798,7 @@
       <c r="D46" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="9" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1707,7 +1811,7 @@
       <c r="D47" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E47" s="9" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1720,7 +1824,7 @@
       <c r="D48" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="9" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1731,31 +1835,31 @@
       <c r="B49" s="4"/>
       <c r="C49" s="5"/>
       <c r="D49" s="7"/>
-      <c r="E49" s="10" t="s">
+      <c r="E49" s="9" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="18"/>
+      <c r="A50" s="16"/>
       <c r="B50" s="2"/>
-      <c r="C50" s="19"/>
+      <c r="C50" s="17"/>
       <c r="D50" s="7"/>
-      <c r="E50" s="20"/>
+      <c r="E50" s="18"/>
     </row>
     <row r="51" spans="1:5" ht="24">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
     </row>
     <row r="52" spans="1:5" ht="17">
       <c r="A52" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E52" s="21" t="s">
+      <c r="E52" s="9" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1763,7 +1867,7 @@
       <c r="A53" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E53" s="21" t="s">
+      <c r="E53" s="9" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1771,7 +1875,7 @@
       <c r="A54" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="E54" s="9" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1779,7 +1883,7 @@
       <c r="A55" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E55" s="21" t="s">
+      <c r="E55" s="9" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1787,7 +1891,7 @@
       <c r="A56" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E56" s="21" t="s">
+      <c r="E56" s="9" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1795,7 +1899,7 @@
       <c r="A57" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E57" s="21" t="s">
+      <c r="E57" s="9" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1803,8 +1907,41 @@
       <c r="A58" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E58" s="21" t="s">
+      <c r="E58" s="9" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="17">
+      <c r="A59" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B59" s="4"/>
+      <c r="E59" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="17">
+      <c r="B60" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="17">
+      <c r="B61" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="17">
+      <c r="B62" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -1817,10 +1954,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A6B2C9D-8306-AC46-BB68-153C3AE89A37}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1833,13 +1970,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
@@ -1869,7 +2006,7 @@
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1877,7 +2014,7 @@
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1885,7 +2022,7 @@
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1893,13 +2030,13 @@
       <c r="A8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="26">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
@@ -1910,7 +2047,7 @@
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" t="s">
         <v>127</v>
       </c>
       <c r="E11" t="s">
@@ -1935,7 +2072,7 @@
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1943,7 +2080,7 @@
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1951,7 +2088,7 @@
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1959,7 +2096,7 @@
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1967,7 +2104,7 @@
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1990,7 +2127,7 @@
       <c r="A22" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" t="s">
         <v>126</v>
       </c>
       <c r="E22" t="s">
@@ -1998,16 +2135,16 @@
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="18"/>
+      <c r="A23" s="16"/>
     </row>
     <row r="24" spans="1:5" ht="26">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
@@ -2050,7 +2187,7 @@
         <v>16</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="22" t="s">
+      <c r="D29" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2067,7 +2204,7 @@
         <v>36</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="22" t="s">
+      <c r="D31" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2077,7 +2214,7 @@
         <v>34</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="22" t="s">
+      <c r="D32" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2087,7 +2224,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="22" t="s">
+      <c r="D33" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2097,7 +2234,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="22" t="s">
+      <c r="D34" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2107,7 +2244,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="22" t="s">
+      <c r="D35" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2178,7 +2315,7 @@
         <v>58</v>
       </c>
       <c r="C42" s="5"/>
-      <c r="D42" s="23"/>
+      <c r="D42" s="19"/>
       <c r="E42" t="s">
         <v>145</v>
       </c>
@@ -2219,7 +2356,7 @@
         <v>47</v>
       </c>
       <c r="C46" s="5"/>
-      <c r="D46" s="22" t="s">
+      <c r="D46" t="s">
         <v>148</v>
       </c>
       <c r="E46" t="s">
@@ -2250,7 +2387,7 @@
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="5"/>
-      <c r="D49" s="22" t="s">
+      <c r="D49" t="s">
         <v>154</v>
       </c>
       <c r="E49" t="s">
@@ -2268,68 +2405,89 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="18"/>
+      <c r="A51" s="16"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="19"/>
+      <c r="C51" s="17"/>
     </row>
     <row r="52" spans="1:5" ht="26">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B53" s="4"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="23"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="19"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B54" s="4"/>
-      <c r="C54" s="19"/>
+      <c r="C54" s="17"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B55" s="4"/>
-      <c r="C55" s="19"/>
+      <c r="C55" s="17"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B56" s="4"/>
-      <c r="C56" s="19"/>
+      <c r="C56" s="17"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B57" s="4"/>
-      <c r="C57" s="19"/>
+      <c r="C57" s="17"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B58" s="4"/>
-      <c r="C58" s="19"/>
+      <c r="C58" s="17"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B59" s="4"/>
-      <c r="C59" s="19"/>
+      <c r="C59" s="17"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B60" s="4"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="B61" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="B62" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="B63" s="4" t="s">
+        <v>235</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2338,10 +2496,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980F6EFD-37CC-F848-B1B5-25B2640236DC}">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2353,13 +2511,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
@@ -2389,7 +2547,7 @@
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" t="s">
         <v>157</v>
       </c>
       <c r="E5" t="s">
@@ -2400,7 +2558,7 @@
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" t="s">
         <v>159</v>
       </c>
       <c r="E6" t="s">
@@ -2411,7 +2569,7 @@
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2419,13 +2577,13 @@
       <c r="A8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="26">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
@@ -2436,7 +2594,6 @@
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="22"/>
       <c r="E11" t="s">
         <v>128</v>
       </c>
@@ -2462,7 +2619,7 @@
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2470,7 +2627,7 @@
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2478,7 +2635,7 @@
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2486,7 +2643,7 @@
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2494,7 +2651,7 @@
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2517,22 +2674,21 @@
       <c r="A22" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="22"/>
       <c r="E22" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="18"/>
+      <c r="A23" s="16"/>
     </row>
     <row r="24" spans="1:5" ht="26">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
@@ -2575,7 +2731,7 @@
         <v>16</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="22" t="s">
+      <c r="D29" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2606,7 +2762,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="22" t="s">
+      <c r="D33" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2638,7 +2794,7 @@
       <c r="C37" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="26" t="s">
+      <c r="D37" s="22" t="s">
         <v>203</v>
       </c>
       <c r="E37" t="s">
@@ -2691,7 +2847,7 @@
         <v>58</v>
       </c>
       <c r="C42" s="5"/>
-      <c r="D42" s="22" t="s">
+      <c r="D42" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2718,7 +2874,7 @@
         <v>46</v>
       </c>
       <c r="C45" s="5"/>
-      <c r="D45" s="22" t="s">
+      <c r="D45" t="s">
         <v>171</v>
       </c>
       <c r="E45" t="s">
@@ -2731,7 +2887,7 @@
         <v>47</v>
       </c>
       <c r="C46" s="5"/>
-      <c r="D46" s="22" t="s">
+      <c r="D46" t="s">
         <v>171</v>
       </c>
       <c r="E46" t="s">
@@ -2769,68 +2925,89 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="18"/>
+      <c r="A50" s="16"/>
       <c r="B50" s="2"/>
-      <c r="C50" s="19"/>
+      <c r="C50" s="17"/>
     </row>
     <row r="51" spans="1:5" ht="26">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B52" s="4"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="23"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="19"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B53" s="4"/>
-      <c r="C53" s="19"/>
+      <c r="C53" s="17"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B54" s="4"/>
-      <c r="C54" s="19"/>
+      <c r="C54" s="17"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B55" s="4"/>
-      <c r="C55" s="19"/>
+      <c r="C55" s="17"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B56" s="4"/>
-      <c r="C56" s="19"/>
+      <c r="C56" s="17"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B57" s="4"/>
-      <c r="C57" s="19"/>
+      <c r="C57" s="17"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B58" s="4"/>
-      <c r="C58" s="19"/>
+      <c r="C58" s="17"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B59" s="4"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="B60" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="B61" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="B62" s="4" t="s">
+        <v>235</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2843,10 +3020,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB83A1CF-D92A-C942-81D6-0796DA3A793F}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2859,13 +3036,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
@@ -2895,7 +3072,7 @@
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2903,7 +3080,7 @@
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2911,19 +3088,18 @@
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="26">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
@@ -2953,7 +3129,7 @@
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2961,7 +3137,7 @@
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" t="s">
         <v>184</v>
       </c>
       <c r="E14" t="s">
@@ -2972,7 +3148,7 @@
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2980,7 +3156,7 @@
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2988,7 +3164,7 @@
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="21" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2996,7 +3172,7 @@
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="21" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3019,22 +3195,21 @@
       <c r="A22" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="22"/>
       <c r="E22" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="18"/>
+      <c r="A23" s="16"/>
     </row>
     <row r="24" spans="1:5" ht="26">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
@@ -3080,7 +3255,7 @@
         <v>16</v>
       </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="22" t="s">
+      <c r="D29" t="s">
         <v>187</v>
       </c>
     </row>
@@ -3090,7 +3265,7 @@
         <v>32</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="22" t="s">
+      <c r="D30" t="s">
         <v>188</v>
       </c>
     </row>
@@ -3100,7 +3275,6 @@
         <v>36</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="22"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3"/>
@@ -3108,7 +3282,7 @@
         <v>34</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="22" t="s">
+      <c r="D32" t="s">
         <v>189</v>
       </c>
     </row>
@@ -3118,7 +3292,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="22" t="s">
+      <c r="D33" t="s">
         <v>190</v>
       </c>
     </row>
@@ -3128,7 +3302,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="22" t="s">
+      <c r="D34" t="s">
         <v>191</v>
       </c>
     </row>
@@ -3138,7 +3312,6 @@
         <v>38</v>
       </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="22"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3"/>
@@ -3154,7 +3327,7 @@
       <c r="C37" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D37" t="s">
         <v>192</v>
       </c>
     </row>
@@ -3164,7 +3337,7 @@
       <c r="C38" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3269,7 +3442,6 @@
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="5"/>
-      <c r="D49" s="22"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3" t="s">
@@ -3282,68 +3454,599 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="18"/>
+      <c r="A51" s="16"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="19"/>
+      <c r="C51" s="17"/>
     </row>
     <row r="52" spans="1:5" ht="26">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B53" s="4"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="23"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="19"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B54" s="4"/>
-      <c r="C54" s="19"/>
+      <c r="C54" s="17"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3" t="s">
         <v>110</v>
       </c>
       <c r="B55" s="4"/>
-      <c r="C55" s="19"/>
+      <c r="C55" s="17"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B56" s="4"/>
-      <c r="C56" s="19"/>
+      <c r="C56" s="17"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B57" s="4"/>
-      <c r="C57" s="19"/>
+      <c r="C57" s="17"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B58" s="4"/>
-      <c r="C58" s="19"/>
+      <c r="C58" s="17"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B59" s="4"/>
-      <c r="C59" s="19"/>
+      <c r="C59" s="17"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B60" s="4"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="B61" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="B62" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="B63" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE750801-3C95-1D4D-A22A-F8144DABC3B9}">
+  <dimension ref="A1:E63"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:B63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="110.1640625" customWidth="1"/>
+    <col min="5" max="5" width="97.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="26">
+      <c r="A1" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="26">
+      <c r="A9" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D22" t="s">
+        <v>222</v>
+      </c>
+      <c r="E22" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="16"/>
+    </row>
+    <row r="25" spans="1:5" ht="26">
+      <c r="A25" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="E27" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="3"/>
+      <c r="B29" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="1"/>
+      <c r="E29" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3"/>
+      <c r="B30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="3"/>
+      <c r="B31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="3"/>
+      <c r="B32" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="3"/>
+      <c r="B33" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="3"/>
+      <c r="B34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="3"/>
+      <c r="B35" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="3"/>
+      <c r="B36" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="3"/>
+      <c r="B37" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="3"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="22"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="3"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="3"/>
+      <c r="B41" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="3"/>
+      <c r="B42" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="3"/>
+      <c r="B43" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="5"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="3"/>
+      <c r="B45" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" s="5"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="3"/>
+      <c r="B46" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" s="5"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="3"/>
+      <c r="B47" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="5"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="3"/>
+      <c r="B48" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" s="5"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="C49" s="5"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" s="4"/>
+      <c r="C50" s="5"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="16"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="17"/>
+    </row>
+    <row r="52" spans="1:5" ht="26">
+      <c r="A52" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="17"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="C54" s="17"/>
+      <c r="D54" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55" s="4"/>
+      <c r="C55" s="17"/>
+      <c r="D55" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="4"/>
+      <c r="C56" s="17"/>
+      <c r="D56" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="4"/>
+      <c r="C57" s="17"/>
+      <c r="D57" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" s="4"/>
+      <c r="C58" s="17"/>
+      <c r="D58" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" s="4"/>
+      <c r="C59" s="17"/>
+      <c r="D59" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B60" s="4"/>
+      <c r="E60" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="B61" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D61" t="s">
+        <v>236</v>
+      </c>
+      <c r="E61" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="B62" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D62" t="s">
+        <v>237</v>
+      </c>
+      <c r="E62" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="B63" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D63" t="s">
+        <v>238</v>
+      </c>
+      <c r="E63" t="s">
+        <v>242</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>